<commit_message>
add 30 Jan to 26 Feb tables
</commit_message>
<xml_diff>
--- a/tables/2023-02/regional_table_Feb.xlsx
+++ b/tables/2023-02/regional_table_Feb.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="77">
   <si>
     <t>Population size</t>
   </si>
@@ -35,12 +35,24 @@
     <t>Proportion sequenced (%)</t>
   </si>
   <si>
+    <t>Omicron (BA.1)</t>
+  </si>
+  <si>
+    <t>Percentage Omicron (BA.1) (95% CI)</t>
+  </si>
+  <si>
     <t>Omicron (BA.2)</t>
   </si>
   <si>
     <t>Percentage Omicron (BA.2) (95% CI)</t>
   </si>
   <si>
+    <t>Omicron (BA.4)</t>
+  </si>
+  <si>
+    <t>Percentage Omicron (BA.4) (95% CI)</t>
+  </si>
+  <si>
     <t>Omicron (BA.5)</t>
   </si>
   <si>
@@ -95,88 +107,142 @@
     <t>11.58</t>
   </si>
   <si>
-    <t>18.07</t>
+    <t>18.09</t>
   </si>
   <si>
     <t>13.17</t>
   </si>
   <si>
-    <t>15.52</t>
+    <t>15.53</t>
   </si>
   <si>
     <t>15.61</t>
   </si>
   <si>
-    <t>1.6</t>
-  </si>
-  <si>
-    <t>3.8</t>
-  </si>
-  <si>
-    <t>1.2</t>
-  </si>
-  <si>
-    <t>0.0</t>
-  </si>
-  <si>
-    <t>0.6</t>
-  </si>
-  <si>
-    <t>5.2</t>
-  </si>
-  <si>
-    <t>5.5 (1.1-15.1)</t>
+    <t>8.8</t>
+  </si>
+  <si>
+    <t>18.0</t>
+  </si>
+  <si>
+    <t>5.8</t>
+  </si>
+  <si>
+    <t>7.8</t>
+  </si>
+  <si>
+    <t>3.0</t>
+  </si>
+  <si>
+    <t>3.3</t>
+  </si>
+  <si>
+    <t>17.7</t>
+  </si>
+  <si>
+    <t>0.3 (0.0-1.8)</t>
   </si>
   <si>
     <t>-</t>
   </si>
   <si>
-    <t>20.0 (0.5-71.6)</t>
-  </si>
-  <si>
-    <t>5.9 (0.1-28.7)</t>
-  </si>
-  <si>
-    <t>52.7 (38.8-66.3)</t>
-  </si>
-  <si>
-    <t>50.0 (29.9-70.1)</t>
-  </si>
-  <si>
-    <t>40.0 (5.3-85.3)</t>
-  </si>
-  <si>
-    <t>83.3 (35.9-99.6)</t>
-  </si>
-  <si>
-    <t>52.9 (27.8-77.0)</t>
-  </si>
-  <si>
-    <t>12.7 (5.3-24.5)</t>
-  </si>
-  <si>
-    <t>3.8 (0.1-19.6)</t>
-  </si>
-  <si>
-    <t>23.5 (6.8-49.9)</t>
-  </si>
-  <si>
-    <t>25.5 (14.7-39.0)</t>
-  </si>
-  <si>
-    <t>38.5 (20.2-59.4)</t>
-  </si>
-  <si>
-    <t>16.7 (0.4-64.1)</t>
-  </si>
-  <si>
-    <t>17.6 (3.8-43.4)</t>
-  </si>
-  <si>
-    <t>3.6 (0.4-12.5)</t>
-  </si>
-  <si>
-    <t>7.7 (0.9-25.1)</t>
+    <t>4.0 (0.1-20.4)</t>
+  </si>
+  <si>
+    <t>8.0 (5.2-11.6)</t>
+  </si>
+  <si>
+    <t>5.7 (2.3-11.4)</t>
+  </si>
+  <si>
+    <t>16.0 (4.5-36.1)</t>
+  </si>
+  <si>
+    <t>10.0 (3.8-20.5)</t>
+  </si>
+  <si>
+    <t>13.9 (4.7-29.5)</t>
+  </si>
+  <si>
+    <t>3.4 (0.4-11.9)</t>
+  </si>
+  <si>
+    <t>0.8 (0.0-4.4)</t>
+  </si>
+  <si>
+    <t>39.3 (33.9-44.9)</t>
+  </si>
+  <si>
+    <t>37.4 (28.8-46.6)</t>
+  </si>
+  <si>
+    <t>40.0 (21.1-61.3)</t>
+  </si>
+  <si>
+    <t>36.7 (24.6-50.1)</t>
+  </si>
+  <si>
+    <t>37.5 (8.5-75.5)</t>
+  </si>
+  <si>
+    <t>52.8 (35.5-69.6)</t>
+  </si>
+  <si>
+    <t>37.9 (25.5-51.6)</t>
+  </si>
+  <si>
+    <t>15.7 (11.8-20.2)</t>
+  </si>
+  <si>
+    <t>12.2 (7.0-19.3)</t>
+  </si>
+  <si>
+    <t>20.0 (10.8-32.3)</t>
+  </si>
+  <si>
+    <t>12.5 (0.3-52.7)</t>
+  </si>
+  <si>
+    <t>11.1 (3.1-26.1)</t>
+  </si>
+  <si>
+    <t>20.7 (11.2-33.4)</t>
+  </si>
+  <si>
+    <t>32.3 (27.1-37.8)</t>
+  </si>
+  <si>
+    <t>41.5 (32.7-50.7)</t>
+  </si>
+  <si>
+    <t>24.0 (9.4-45.1)</t>
+  </si>
+  <si>
+    <t>25.0 (14.7-37.9)</t>
+  </si>
+  <si>
+    <t>50.0 (15.7-84.3)</t>
+  </si>
+  <si>
+    <t>16.7 (6.4-32.8)</t>
+  </si>
+  <si>
+    <t>32.8 (21.0-46.3)</t>
+  </si>
+  <si>
+    <t>4.2 (2.2-7.0)</t>
+  </si>
+  <si>
+    <t>2.4 (0.5-7.0)</t>
+  </si>
+  <si>
+    <t>8.3 (2.8-18.4)</t>
+  </si>
+  <si>
+    <t>5.6 (0.7-18.7)</t>
+  </si>
+  <si>
+    <t>5.2 (1.1-14.4)</t>
   </si>
 </sst>
 </file>
@@ -280,66 +346,90 @@
       <c r="R1" t="s">
         <v>16</v>
       </c>
+      <c r="S1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B2" t="n">
         <v>8738791.0</v>
       </c>
       <c r="C2" t="n">
-        <v>3546.0</v>
+        <v>3549.0</v>
       </c>
       <c r="D2" t="n">
-        <v>32463.0</v>
+        <v>32466.0</v>
       </c>
       <c r="E2" t="n">
-        <v>371.0</v>
+        <v>372.0</v>
       </c>
       <c r="F2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="G2" t="n">
-        <v>55.0</v>
+        <v>313.0</v>
       </c>
       <c r="H2" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="I2" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="J2" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="K2" t="n">
-        <v>29.0</v>
+        <v>25.0</v>
       </c>
       <c r="L2" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="M2" t="n">
-        <v>7.0</v>
+        <v>1.0</v>
       </c>
       <c r="N2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="O2" t="n">
-        <v>14.0</v>
+        <v>123.0</v>
       </c>
       <c r="P2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="Q2" t="n">
-        <v>2.0</v>
+        <v>49.0</v>
       </c>
       <c r="R2" t="s">
-        <v>53</v>
+        <v>59</v>
+      </c>
+      <c r="S2" t="n">
+        <v>101.0</v>
+      </c>
+      <c r="T2" t="s">
+        <v>65</v>
+      </c>
+      <c r="U2" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="V2" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B3" t="n">
         <v>1861791.0</v>
@@ -354,48 +444,60 @@
         <v>550.0</v>
       </c>
       <c r="F3" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="G3" t="n">
-        <v>26.0</v>
+        <v>123.0</v>
       </c>
       <c r="H3" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="I3" t="n">
         <v>0.0</v>
       </c>
       <c r="J3" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="K3" t="n">
-        <v>13.0</v>
+        <v>7.0</v>
       </c>
       <c r="L3" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="M3" t="n">
         <v>1.0</v>
       </c>
       <c r="N3" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="O3" t="n">
-        <v>10.0</v>
+        <v>46.0</v>
       </c>
       <c r="P3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="Q3" t="n">
-        <v>2.0</v>
+        <v>15.0</v>
       </c>
       <c r="R3" t="s">
-        <v>54</v>
+        <v>60</v>
+      </c>
+      <c r="S3" t="n">
+        <v>51.0</v>
+      </c>
+      <c r="T3" t="s">
+        <v>66</v>
+      </c>
+      <c r="U3" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="V3" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B4" t="n">
         <v>1451080.0</v>
@@ -410,110 +512,134 @@
         <v>308.0</v>
       </c>
       <c r="F4" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="G4" t="n">
-        <v>5.0</v>
+        <v>25.0</v>
       </c>
       <c r="H4" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="I4" t="n">
         <v>1.0</v>
       </c>
       <c r="J4" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="K4" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="L4" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="M4" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="N4" t="s">
         <v>43</v>
       </c>
       <c r="O4" t="n">
-        <v>0.0</v>
+        <v>10.0</v>
       </c>
       <c r="P4" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="R4" t="s">
-        <v>38</v>
+        <v>47</v>
+      </c>
+      <c r="S4" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="T4" t="s">
+        <v>67</v>
+      </c>
+      <c r="U4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V4" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B5" t="n">
         <v>1472184.0</v>
       </c>
       <c r="C5" t="n">
-        <v>765.0</v>
+        <v>766.0</v>
       </c>
       <c r="D5" t="n">
-        <v>5207.0</v>
+        <v>5208.0</v>
       </c>
       <c r="E5" t="n">
         <v>354.0</v>
       </c>
       <c r="F5" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0</v>
+        <v>60.0</v>
       </c>
       <c r="H5" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="I5" t="n">
         <v>0.0</v>
       </c>
       <c r="J5" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="K5" t="n">
-        <v>0.0</v>
+        <v>6.0</v>
       </c>
       <c r="L5" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="M5" t="n">
         <v>0.0</v>
       </c>
       <c r="N5" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="O5" t="n">
-        <v>0.0</v>
+        <v>22.0</v>
       </c>
       <c r="P5" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.0</v>
+        <v>12.0</v>
       </c>
       <c r="R5" t="s">
-        <v>38</v>
+        <v>61</v>
+      </c>
+      <c r="S5" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="T5" t="s">
+        <v>68</v>
+      </c>
+      <c r="U5" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="V5" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B6" t="n">
         <v>833178.0</v>
       </c>
       <c r="C6" t="n">
-        <v>262.0</v>
+        <v>263.0</v>
       </c>
       <c r="D6" t="n">
         <v>2179.0</v>
@@ -522,104 +648,128 @@
         <v>262.0</v>
       </c>
       <c r="F6" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="G6" t="n">
-        <v>0.0</v>
+        <v>8.0</v>
       </c>
       <c r="H6" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="I6" t="n">
         <v>0.0</v>
       </c>
       <c r="J6" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="K6" t="n">
         <v>0.0</v>
       </c>
       <c r="L6" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="M6" t="n">
         <v>0.0</v>
       </c>
       <c r="N6" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="O6" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="P6" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="R6" t="s">
-        <v>38</v>
+        <v>62</v>
+      </c>
+      <c r="S6" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="T6" t="s">
+        <v>69</v>
+      </c>
+      <c r="U6" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V6" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B7" t="n">
         <v>2567001.0</v>
       </c>
       <c r="C7" t="n">
-        <v>1078.0</v>
+        <v>1079.0</v>
       </c>
       <c r="D7" t="n">
-        <v>7904.0</v>
+        <v>7906.0</v>
       </c>
       <c r="E7" t="n">
         <v>308.0</v>
       </c>
       <c r="F7" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="G7" t="n">
-        <v>6.0</v>
+        <v>36.0</v>
       </c>
       <c r="H7" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="I7" t="n">
         <v>0.0</v>
       </c>
       <c r="J7" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="K7" t="n">
         <v>5.0</v>
       </c>
       <c r="L7" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="M7" t="n">
         <v>0.0</v>
       </c>
       <c r="N7" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="O7" t="n">
-        <v>1.0</v>
+        <v>19.0</v>
       </c>
       <c r="P7" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="R7" t="s">
-        <v>38</v>
+        <v>63</v>
+      </c>
+      <c r="S7" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="T7" t="s">
+        <v>70</v>
+      </c>
+      <c r="U7" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="V7" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B8" t="n">
         <v>553557.0</v>
@@ -634,43 +784,55 @@
         <v>446.0</v>
       </c>
       <c r="F8" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="G8" t="n">
-        <v>17.0</v>
+        <v>58.0</v>
       </c>
       <c r="H8" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="I8" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="J8" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="K8" t="n">
-        <v>9.0</v>
+        <v>2.0</v>
       </c>
       <c r="L8" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="M8" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="N8" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="O8" t="n">
+        <v>22.0</v>
+      </c>
+      <c r="P8" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="R8" t="s">
+        <v>64</v>
+      </c>
+      <c r="S8" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="T8" t="s">
+        <v>71</v>
+      </c>
+      <c r="U8" t="n">
         <v>3.0</v>
       </c>
-      <c r="P8" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q8" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="R8" t="s">
-        <v>38</v>
+      <c r="V8" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>